<commit_message>
Add one more test to QA
</commit_message>
<xml_diff>
--- a/documentation/QA_Cryo.xlsx
+++ b/documentation/QA_Cryo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viki\Pictures\Вики презентации\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viki\Documents\GitHub\Cryo\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A54A2A-D40A-491F-96FD-563383621EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5065C4A9-0868-4E7F-8D93-A415DD68BB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{A6D4AAB8-A785-4009-A828-6DCDF3FD03C5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
   <si>
     <t>№</t>
   </si>
@@ -111,6 +111,18 @@
   </si>
   <si>
     <t>TC_01</t>
+  </si>
+  <si>
+    <t>Test case 5</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>Testing the digital will form</t>
+  </si>
+  <si>
+    <t>Things can be added</t>
   </si>
 </sst>
 </file>
@@ -272,9 +284,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -285,6 +294,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -300,10 +315,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -621,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F36BE0-5BE2-40E2-A04F-0A11F522939B}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -637,78 +649,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>1</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -716,85 +728,85 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>2</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -802,85 +814,85 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A23" s="5">
+      <c r="A23" s="4">
         <v>3</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -888,85 +900,85 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A31" s="5">
+      <c r="A31" s="4">
         <v>4</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -974,18 +986,97 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:5" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="A33" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39" s="4">
+        <v>5</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A33:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>